<commit_message>
test: Check p-values are in (0,1)
</commit_message>
<xml_diff>
--- a/tests/snp_validator.xlsx
+++ b/tests/snp_validator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karatugo/Documents/GitHub/gwas-assoc-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD31092E-1900-BA44-9FCA-5D7669CB90C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCE6E37-9378-AE43-BC59-0AE74EA8DF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9660" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="1300" windowWidth="29060" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="183">
   <si>
     <t>A unique free-text label for each genome-wide association study in the publication</t>
   </si>
@@ -597,7 +597,16 @@
     <t>black</t>
   </si>
   <si>
-    <t>rs2</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>no-rsid-val</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>1E-5</t>
   </si>
 </sst>
 </file>
@@ -1420,12 +1429,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1593,12 +1602,29 @@
         <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Sorry, values must be less than 255 characters. Please try again." prompt="Values must be less than 255 characters" sqref="M5:M1001 D5:G1001 A5:B1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Sorry, values must be less than 255 characters. Please try again." prompt="Values must be less than 255 characters" sqref="A5:B1001 D5:G1001 M5:M1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
test: Check beta and OR are float and OR > 0
</commit_message>
<xml_diff>
--- a/tests/snp_validator.xlsx
+++ b/tests/snp_validator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karatugo/Documents/GitHub/gwas-assoc-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCE6E37-9378-AE43-BC59-0AE74EA8DF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C30AE3-3C90-C44B-97FC-3281CE512DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="1300" windowWidth="29060" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="5600" windowWidth="29180" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="188">
   <si>
     <t>A unique free-text label for each genome-wide association study in the publication</t>
   </si>
@@ -607,6 +607,21 @@
   </si>
   <si>
     <t>1E-5</t>
+  </si>
+  <si>
+    <t>rs4650718</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>not-float</t>
+  </si>
+  <si>
+    <t>rs4650719</t>
+  </si>
+  <si>
+    <t>rs4650720</t>
   </si>
 </sst>
 </file>
@@ -1429,12 +1444,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1622,9 +1637,60 @@
         <v>181</v>
       </c>
     </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Sorry, values must be less than 255 characters. Please try again." prompt="Values must be less than 255 characters" sqref="A5:B1001 D5:G1001 M5:M1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Sorry, values must be less than 255 characters. Please try again." prompt="Values must be less than 255 characters" sqref="M5:M1001 D5:G1001 A5:B1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>